<commit_message>
kernel 1 en 2 voor assignment 3
</commit_message>
<xml_diff>
--- a/TSE/Assignment 2/Timing Mandelbrot.xlsx
+++ b/TSE/Assignment 2/Timing Mandelbrot.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="16925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17329"/>
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tim\Documents\GitHub\S6T\TSE\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tim\Documents\GitHub\S6T\TSE\Assignment 2\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="12">
   <si>
     <t>CPU</t>
   </si>
@@ -57,6 +57,9 @@
   </si>
   <si>
     <t>TIME (msec)</t>
+  </si>
+  <si>
+    <t>TIME (TOTAL)</t>
   </si>
 </sst>
 </file>
@@ -414,10 +417,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q17"/>
+  <dimension ref="A1:R17"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="Q18" sqref="Q18"/>
+      <selection activeCell="R18" sqref="R18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -439,10 +442,11 @@
     <col min="15" max="15" width="16.6640625" style="1" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="17" style="1" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="10.109375" style="1" customWidth="1"/>
-    <col min="18" max="16384" width="9.109375" style="1"/>
+    <col min="18" max="18" width="12.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="19" max="16384" width="9.109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -450,7 +454,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -499,8 +503,11 @@
       <c r="Q2" s="1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="R2" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>800</v>
       </c>
@@ -549,8 +556,11 @@
       <c r="Q3" s="1">
         <v>2.6100000000000002E-2</v>
       </c>
-    </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="R3" s="1">
+        <v>114.11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>1024</v>
       </c>
@@ -599,8 +609,11 @@
       <c r="Q4" s="1">
         <v>1.7100000000000001E-2</v>
       </c>
-    </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="R4" s="1">
+        <v>129.91</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>1280</v>
       </c>
@@ -649,8 +662,11 @@
       <c r="Q5" s="1">
         <v>1.84E-2</v>
       </c>
-    </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="R5" s="1">
+        <v>122.11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>1600</v>
       </c>
@@ -699,8 +715,11 @@
       <c r="Q6" s="1">
         <v>1.9199999999999998E-2</v>
       </c>
-    </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="R6" s="1">
+        <v>144.16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>1920</v>
       </c>
@@ -749,8 +768,11 @@
       <c r="Q7" s="1">
         <v>2.6499999999999999E-2</v>
       </c>
-    </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="R7" s="1">
+        <v>115.69</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>1920</v>
       </c>
@@ -799,8 +821,11 @@
       <c r="Q8" s="1">
         <v>1.9699999999999999E-2</v>
       </c>
-    </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="R8" s="1">
+        <v>224.89</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>1920</v>
       </c>
@@ -849,8 +874,11 @@
       <c r="Q9" s="1">
         <v>2.2700000000000001E-2</v>
       </c>
-    </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="R9" s="1">
+        <v>164.03</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <v>1920</v>
       </c>
@@ -899,8 +927,11 @@
       <c r="Q10" s="1">
         <v>3.1600000000000003E-2</v>
       </c>
-    </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="R10" s="1">
+        <v>145.1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
         <v>1920</v>
       </c>
@@ -949,8 +980,11 @@
       <c r="Q11" s="1">
         <v>2.2200000000000001E-2</v>
       </c>
-    </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="R11" s="1">
+        <v>123.16</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
         <v>3840</v>
       </c>
@@ -999,8 +1033,11 @@
       <c r="Q12" s="1">
         <v>1.8800000000000001E-2</v>
       </c>
-    </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="R12" s="1">
+        <v>1062.8599999999999</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
         <v>3840</v>
       </c>
@@ -1049,8 +1086,11 @@
       <c r="Q13" s="1">
         <v>2.0500000000000001E-2</v>
       </c>
-    </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="R13" s="1">
+        <v>126.04</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
         <v>3840</v>
       </c>
@@ -1099,8 +1139,11 @@
       <c r="Q14" s="1">
         <v>2.2200000000000001E-2</v>
       </c>
-    </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="R14" s="1">
+        <v>152.88999999999999</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
         <v>3840</v>
       </c>
@@ -1149,8 +1192,11 @@
       <c r="Q15" s="1">
         <v>1.7100000000000001E-2</v>
       </c>
-    </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="R15" s="1">
+        <v>137.46</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
         <v>3840</v>
       </c>
@@ -1199,8 +1245,11 @@
       <c r="Q16" s="1">
         <v>1.7999999999999999E-2</v>
       </c>
-    </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="R16" s="1">
+        <v>1033.0899999999999</v>
+      </c>
+    </row>
+    <row r="17" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A17" s="1">
         <v>3840</v>
       </c>
@@ -1248,6 +1297,9 @@
       </c>
       <c r="Q17" s="1">
         <v>1.8800000000000001E-2</v>
+      </c>
+      <c r="R17" s="1">
+        <v>1083.43</v>
       </c>
     </row>
   </sheetData>

</xml_diff>